<commit_message>
One error, but mostly done
</commit_message>
<xml_diff>
--- a/Test_screen.xlsx
+++ b/Test_screen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,9 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>US,N/A</t>
   </si>
   <si>
@@ -172,57 +175,9 @@
     <t>05-05-2028</t>
   </si>
   <si>
-    <t>22-04-2024 12:26:33</t>
-  </si>
-  <si>
-    <t>12-02-2024 12:00:21</t>
-  </si>
-  <si>
-    <t>12-02-2024 12:00:19</t>
-  </si>
-  <si>
-    <t>12-02-2024 08:35:18</t>
-  </si>
-  <si>
-    <t>12-02-2024 08:35:15</t>
-  </si>
-  <si>
-    <t>01-02-2024 14:40:38</t>
-  </si>
-  <si>
-    <t>29-04-2024 16:14:34</t>
-  </si>
-  <si>
-    <t>22-04-2024 12:27:00</t>
-  </si>
-  <si>
     <t>sylvia.ingle</t>
   </si>
   <si>
-    <t>22-04-2024 13:16:15</t>
-  </si>
-  <si>
-    <t>12-02-2024 12:00:22</t>
-  </si>
-  <si>
-    <t>12-02-2024 12:00:20</t>
-  </si>
-  <si>
-    <t>12-02-2024 08:35:19</t>
-  </si>
-  <si>
-    <t>12-02-2024 08:35:16</t>
-  </si>
-  <si>
-    <t>01-02-2024 15:33:12</t>
-  </si>
-  <si>
-    <t>29-04-2024 16:17:27</t>
-  </si>
-  <si>
-    <t>22-04-2024 12:27:07</t>
-  </si>
-  <si>
     <t>12-05-2026</t>
   </si>
   <si>
@@ -230,6 +185,9 @@
   </si>
   <si>
     <t>02-02-2025</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>United Kingdom</t>
@@ -726,29 +684,32 @@
       <c r="F2" t="s">
         <v>44</v>
       </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
       <c r="I2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="J2" s="2">
+        <v>45404.5184375</v>
+      </c>
+      <c r="M2" s="2">
+        <v>45404.55295138889</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="R2" t="s">
+        <v>57</v>
       </c>
       <c r="T2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="V2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="W2" s="2">
         <v>45404.55295138889</v>
@@ -774,28 +735,28 @@
         <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" t="s">
-        <v>62</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="J3" s="2">
+        <v>45334.50024305555</v>
+      </c>
+      <c r="M3" s="2">
+        <v>45334.50025462963</v>
+      </c>
+      <c r="R3" t="s">
+        <v>57</v>
       </c>
       <c r="T3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="V3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="W3" s="2">
         <v>45334.50025462963</v>
@@ -818,28 +779,28 @@
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" t="s">
-        <v>63</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="J4" s="2">
+        <v>45334.50021990741</v>
+      </c>
+      <c r="M4" s="2">
+        <v>45334.50023148148</v>
+      </c>
+      <c r="R4" t="s">
+        <v>57</v>
       </c>
       <c r="T4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="V4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="W4" s="2">
         <v>45334.50023148148</v>
@@ -865,28 +826,28 @@
         <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="J5" s="2">
+        <v>45334.35784722222</v>
+      </c>
+      <c r="M5" s="2">
+        <v>45334.3578587963</v>
+      </c>
+      <c r="R5" t="s">
+        <v>57</v>
       </c>
       <c r="T5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="V5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="W5" s="2">
         <v>45334.3578587963</v>
@@ -912,28 +873,28 @@
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="J6" s="2">
+        <v>45334.3578125</v>
+      </c>
+      <c r="M6" s="2">
+        <v>45334.35782407408</v>
+      </c>
+      <c r="R6" t="s">
+        <v>57</v>
       </c>
       <c r="T6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U6" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="V6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="W6" s="2">
         <v>45334.35782407408</v>
@@ -952,23 +913,23 @@
       <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2">
+        <v>45323.61155092593</v>
+      </c>
+      <c r="M7" s="2">
+        <v>45323.64805555555</v>
+      </c>
+      <c r="R7" t="s">
         <v>57</v>
       </c>
-      <c r="M7" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
       <c r="T7" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="U7" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="V7" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="W7" s="2">
         <v>45323.64805555555</v>
@@ -990,47 +951,50 @@
       <c r="E8" t="s">
         <v>43</v>
       </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="J8" s="2">
+        <v>45411.6767824074</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
-      </c>
-      <c r="M8" t="s">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="M8" s="2">
+        <v>45411.67878472222</v>
       </c>
       <c r="N8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="O8" t="s">
-        <v>60</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="R8" t="s">
+        <v>57</v>
       </c>
       <c r="T8" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="U8" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="V8" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="W8" s="2">
         <v>45411.67878472222</v>
       </c>
       <c r="X8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1052,29 +1016,32 @@
       <c r="F9" t="s">
         <v>44</v>
       </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
       <c r="I9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="2">
+        <v>45404.51875</v>
+      </c>
+      <c r="M9" s="2">
+        <v>45404.51883101852</v>
+      </c>
+      <c r="N9" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T9" t="s">
         <v>59</v>
       </c>
-      <c r="M9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N9" t="s">
-        <v>71</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>73</v>
-      </c>
       <c r="U9" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="V9" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="W9" s="2">
         <v>45404.51883101852</v>

</xml_diff>